<commit_message>
ajuste a la vista
</commit_message>
<xml_diff>
--- a/ejemplo_import.xlsx
+++ b/ejemplo_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyecto_inventario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C7EB82-5946-4B0B-8432-7969398A6D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441C9339-7FBD-4681-ABE3-A1F1E2A1F300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB2731EC-79FC-49A3-8460-AA72F3E7A367}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{EB2731EC-79FC-49A3-8460-AA72F3E7A367}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,32 +36,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>nombre_producto</t>
   </si>
   <si>
-    <t>cku</t>
-  </si>
-  <si>
     <t>categoria</t>
   </si>
   <si>
     <t>imagen</t>
   </si>
   <si>
-    <t>precio_general</t>
-  </si>
-  <si>
-    <t>precio_empresa</t>
-  </si>
-  <si>
     <t>descripcion</t>
   </si>
   <si>
-    <t>en_regalo</t>
-  </si>
-  <si>
     <t>descuento</t>
   </si>
   <si>
@@ -80,28 +68,58 @@
     <t>dias_garantia</t>
   </si>
   <si>
-    <t>unidad_almacen</t>
-  </si>
-  <si>
-    <t>almacen</t>
-  </si>
-  <si>
-    <t>stock_almacen</t>
-  </si>
-  <si>
     <t>umbral</t>
   </si>
   <si>
-    <t>sucursal</t>
-  </si>
-  <si>
-    <t>unidad_precio</t>
-  </si>
-  <si>
-    <t>tipo_cliente</t>
-  </si>
-  <si>
     <t>precio</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>bodega</t>
+  </si>
+  <si>
+    <t>ces</t>
+  </si>
+  <si>
+    <t>unidad_bodega</t>
+  </si>
+  <si>
+    <t>CASE ASUS TUF GAMING GT301 ATX MID-TOWER VIDRIO TEMPLADO RGB</t>
+  </si>
+  <si>
+    <t>TUF GAMING GT301</t>
+  </si>
+  <si>
+    <t>CASE</t>
+  </si>
+  <si>
+    <t>https://compuvisionperu.pe/public/img/productos/MCNo6oqOD0OacJkAmtUR82D46SHvxYE9bRoY6UnAL1bnBBoov95t19oxRvjEKnEm5sB2Co3NgU1hWgMI.jpg</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor, sit amet consectetur adipisicing elit. Vero, tempore? Voluptatem velit laborum nisi cumque qui ullam sunt nulla enim distinctio tenetur aliquid</t>
+  </si>
+  <si>
+    <t>SUJETO A IMPUESTO</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Almacen A</t>
+  </si>
+  <si>
+    <t>Cali</t>
+  </si>
+  <si>
+    <t>NO ATENDER SIN STOCK</t>
   </si>
 </sst>
 </file>
@@ -163,30 +181,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC0FDCA4-BF5E-41F0-8BD9-866AF4D39EA8}" name="Tabla1" displayName="Tabla1" ref="A1:V3" totalsRowShown="0">
-  <autoFilter ref="A1:V3" xr:uid="{CC0FDCA4-BF5E-41F0-8BD9-866AF4D39EA8}"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC0FDCA4-BF5E-41F0-8BD9-866AF4D39EA8}" name="Tabla1" displayName="Tabla1" ref="A1:Q3" totalsRowShown="0">
+  <autoFilter ref="A1:Q3" xr:uid="{CC0FDCA4-BF5E-41F0-8BD9-866AF4D39EA8}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{25A9D712-99D2-4B8C-8037-6842D1087D50}" name="nombre_producto"/>
-    <tableColumn id="2" xr3:uid="{19910199-9C42-4228-82E4-84843975677B}" name="cku"/>
+    <tableColumn id="2" xr3:uid="{19910199-9C42-4228-82E4-84843975677B}" name="codigo"/>
     <tableColumn id="3" xr3:uid="{6190BE4B-4DE4-41B8-AB92-64FB4B09D802}" name="categoria"/>
     <tableColumn id="4" xr3:uid="{E3788859-5006-4EFD-A88B-6EFCCC105BB3}" name="imagen"/>
-    <tableColumn id="5" xr3:uid="{12F03375-415A-4740-9B6D-3C049ED7431F}" name="precio_general"/>
-    <tableColumn id="6" xr3:uid="{364B4D2F-3E1F-46B1-8428-DB7910229692}" name="precio_empresa"/>
     <tableColumn id="7" xr3:uid="{E38E76ED-350A-4018-9345-9A0C4607DD95}" name="descripcion"/>
-    <tableColumn id="8" xr3:uid="{903B5573-DAFB-46F0-9468-A3281223C7D2}" name="en_regalo"/>
     <tableColumn id="9" xr3:uid="{DE1CF66E-C4CC-4471-B00C-6CBBD1B19C21}" name="descuento"/>
     <tableColumn id="10" xr3:uid="{62508C99-0CF5-40B2-A56E-7C0F3CEDE810}" name="tipo_impuesto"/>
     <tableColumn id="11" xr3:uid="{411B867F-CB25-495C-9120-1C5E6F061059}" name="importe_iva"/>
-    <tableColumn id="13" xr3:uid="{0EBF6D2B-5B96-42D0-8706-BFE2C9183594}" name="disponibilidad"/>
+    <tableColumn id="13" xr3:uid="{0EBF6D2B-5B96-42D0-8706-BFE2C9183594}" name="estado"/>
     <tableColumn id="14" xr3:uid="{1A5DF606-D706-4846-9003-BC2AF66253E2}" name="dias_garantia"/>
-    <tableColumn id="12" xr3:uid="{9216C4A6-190A-4E92-B644-6BCEB4FEED74}" name="estado"/>
-    <tableColumn id="15" xr3:uid="{638AA2B5-5845-45F4-96EE-B40FA8469758}" name="unidad_almacen"/>
-    <tableColumn id="16" xr3:uid="{6B48D4B8-2741-444F-B253-2CA001499C5D}" name="almacen"/>
-    <tableColumn id="17" xr3:uid="{439F6A55-9C16-49FB-AB9A-A09A99EDF5D7}" name="stock_almacen"/>
+    <tableColumn id="12" xr3:uid="{9216C4A6-190A-4E92-B644-6BCEB4FEED74}" name="disponibilidad"/>
+    <tableColumn id="15" xr3:uid="{638AA2B5-5845-45F4-96EE-B40FA8469758}" name="unidad_bodega"/>
+    <tableColumn id="16" xr3:uid="{6B48D4B8-2741-444F-B253-2CA001499C5D}" name="bodega"/>
+    <tableColumn id="17" xr3:uid="{439F6A55-9C16-49FB-AB9A-A09A99EDF5D7}" name="stock"/>
     <tableColumn id="18" xr3:uid="{62443A68-5AB2-4693-9C90-CE731747F227}" name="umbral"/>
-    <tableColumn id="19" xr3:uid="{7389DABD-850C-4413-A3FC-3DE400E9AAC8}" name="sucursal"/>
-    <tableColumn id="20" xr3:uid="{3C2DB0B7-0D50-4507-AC69-4A34C396F9A4}" name="unidad_precio"/>
-    <tableColumn id="21" xr3:uid="{5763AEF9-3F63-4F36-998D-F0ED846B93B0}" name="tipo_cliente"/>
+    <tableColumn id="19" xr3:uid="{7389DABD-850C-4413-A3FC-3DE400E9AAC8}" name="ces"/>
     <tableColumn id="22" xr3:uid="{B2351F0E-277F-441A-8FCE-53E3BDF3EF6C}" name="precio"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -510,55 +523,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CC37DA-9E92-4D9A-A160-189FBD80FE0C}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="13" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" customWidth="1"/>
-    <col min="20" max="20" width="16" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="8" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -567,40 +575,75 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="E2" t="s">
         <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>